<commit_message>
Artefato 17 finalizado correcoes no 16 e 15
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t xml:space="preserve">Externo</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">(x)1</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerencia emite ordem de produção</t>
+    <t xml:space="preserve">Gerencia emite ordem de produção </t>
   </si>
   <si>
     <t xml:space="preserve">(x)2</t>
@@ -88,55 +88,103 @@
     <t xml:space="preserve">Gerencia envia ordem de produção</t>
   </si>
   <si>
-    <t xml:space="preserve">(4)x</t>
+    <t xml:space="preserve">(x)3</t>
   </si>
   <si>
     <t xml:space="preserve">Linha de produção pega componentes necessários</t>
   </si>
   <si>
-    <t xml:space="preserve">(5) x</t>
+    <t xml:space="preserve">(x)4</t>
   </si>
   <si>
     <t xml:space="preserve">Linha de produção seleciona componentes a serem fixados</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linha de produção confere  componentes fixados</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linha de produção separa subcomponente </t>
   </si>
   <si>
+    <t xml:space="preserve">(x)7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testar subcomponentes</t>
   </si>
   <si>
     <t xml:space="preserve">Linha de produção envia subcomponente não testado</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Controle de Qualidade separa componente para teste</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Montar a maquina</t>
   </si>
   <si>
     <t xml:space="preserve">Linha de produção recebe  subcomponentes testados</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linha de produção coloca subcomponentes testados</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linha de produção termina montagem da maquina</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linha de produção seleciona maquina montada</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entregar maquina</t>
   </si>
   <si>
     <t xml:space="preserve">Controle de Qualidade envia maquina</t>
   </si>
   <si>
+    <t xml:space="preserve">(x)14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerencia separa maquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(x)15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priorizar pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negocios envia pedido de prioridade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerencia separa pedido a priorizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(x)17</t>
   </si>
 </sst>
 </file>
@@ -204,7 +252,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +301,18 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF55308D"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF4000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -295,7 +355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -309,7 +369,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -321,7 +381,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -376,10 +436,18 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +462,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -461,7 +541,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF55308D"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -475,11 +555,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
@@ -568,11 +648,11 @@
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="15"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="14"/>
@@ -586,11 +666,11 @@
       <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="15"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="14"/>
@@ -622,7 +702,7 @@
       <c r="D7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="20" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="12"/>
@@ -640,11 +720,11 @@
       <c r="D8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="14"/>
@@ -660,7 +740,9 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="14"/>
@@ -672,11 +754,13 @@
         <v>7</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
@@ -688,11 +772,13 @@
         <v>8</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="23" t="s">
+        <v>30</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
@@ -706,14 +792,14 @@
       <c r="D12" s="19"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
-        <v>28</v>
+      <c r="A13" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
@@ -721,10 +807,12 @@
       <c r="C13" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="11"/>
+      <c r="D13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -732,30 +820,32 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>30</v>
+      <c r="D14" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="13"/>
@@ -764,8 +854,8 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
-        <v>31</v>
+      <c r="A16" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>12</v>
@@ -774,18 +864,20 @@
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
-        <v>31</v>
+      <c r="A17" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>12</v>
@@ -794,18 +886,20 @@
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="s">
-        <v>31</v>
+      <c r="A18" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>12</v>
@@ -814,18 +908,20 @@
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
-        <v>31</v>
+      <c r="A19" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>12</v>
@@ -834,28 +930,26 @@
         <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="18" t="n">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="13"/>
@@ -863,37 +957,126 @@
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="s">
-        <v>31</v>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="18" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="27"/>
+      <c r="B23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="18" t="n">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28"/>
+      <c r="B26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+    </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="29"/>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -903,7 +1086,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
@@ -913,10 +1096,12 @@
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A16:A20"/>
     <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correcoes nos artefatos 15,16,17 e comeco do 18
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
@@ -175,7 +175,7 @@
     <t xml:space="preserve">Priorizar pedido</t>
   </si>
   <si>
-    <t xml:space="preserve">Negocios envia pedido de prioridade</t>
+    <t xml:space="preserve">Negócios envia pedido de prioridade</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -195,7 +195,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -233,19 +233,52 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="7.5"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="7.5"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -355,7 +388,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,7 +402,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -381,7 +414,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -404,56 +437,80 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -556,10 +613,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
@@ -567,7 +624,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14"/>
   </cols>
   <sheetData>
@@ -681,48 +739,48 @@
         <v>19</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="25" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="13"/>
@@ -730,17 +788,17 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="18" t="n">
+      <c r="C9" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="26" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="13"/>
@@ -748,17 +806,17 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="18" t="n">
+      <c r="C10" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="21" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="26" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="13"/>
@@ -766,17 +824,17 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="18" t="n">
+      <c r="C11" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="26" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="13"/>
@@ -784,33 +842,33 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="18" t="n">
+      <c r="C13" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="22" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="11"/>
@@ -820,19 +878,19 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="18" t="n">
+      <c r="C14" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="25" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="13"/>
@@ -840,12 +898,12 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="13"/>
@@ -854,21 +912,21 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="18" t="n">
+      <c r="C16" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="30" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="25" t="s">
         <v>38</v>
       </c>
       <c r="H16" s="13"/>
@@ -876,21 +934,21 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="18" t="n">
+      <c r="C17" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="30" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="25" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="13"/>
@@ -898,21 +956,21 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C18" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="30" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="25" t="s">
         <v>42</v>
       </c>
       <c r="H18" s="13"/>
@@ -920,21 +978,21 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="18" t="n">
+      <c r="C19" s="20" t="n">
         <v>14</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="13"/>
@@ -942,13 +1000,13 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="1"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -958,19 +1016,19 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="18" t="n">
+      <c r="C21" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="11"/>
@@ -980,21 +1038,21 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="20" t="n">
         <v>16</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="30" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="25" t="s">
         <v>49</v>
       </c>
       <c r="H22" s="13"/>
@@ -1002,11 +1060,11 @@
       <c r="J22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="1"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -1016,20 +1074,20 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="34" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="18" t="n">
+      <c r="C24" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="30" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="11"/>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="22" t="s">
         <v>52</v>
       </c>
       <c r="G24" s="13"/>
@@ -1038,17 +1096,17 @@
       <c r="J24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="20" t="n">
         <v>18</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="30" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="25" t="s">
         <v>54</v>
       </c>
       <c r="H25" s="13"/>
@@ -1056,11 +1114,11 @@
       <c r="J25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="18"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="1"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -1071,7 +1129,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="29"/>
+      <c r="D28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Altera~coes nos artefatos e artefato 18 concluido
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
@@ -402,7 +402,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -414,7 +414,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -612,11 +612,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>

</xml_diff>

<commit_message>
aretfatos 18 e 19 para pdf
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
@@ -67,13 +67,13 @@
     <t xml:space="preserve">(x)</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerencia verifica solicitação de produção</t>
+    <t xml:space="preserve">Gerencia separa solicitação de produção</t>
   </si>
   <si>
     <t xml:space="preserve">(x)1</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerencia emite ordem de produção </t>
+    <t xml:space="preserve">Gerencia insere solicitação de produção</t>
   </si>
   <si>
     <t xml:space="preserve">(x)2</t>
@@ -402,7 +402,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -414,7 +414,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -613,13 +613,13 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.22"/>

</xml_diff>

<commit_message>
Mudanças no artefato 18 17 16
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário - Página1-convertido.xlsx
@@ -91,13 +91,13 @@
     <t xml:space="preserve">(x)3</t>
   </si>
   <si>
-    <t xml:space="preserve">Linha de produção pega componentes necessários</t>
+    <t xml:space="preserve">Linha de produção confere ordem de produção</t>
   </si>
   <si>
     <t xml:space="preserve">(x)4</t>
   </si>
   <si>
-    <t xml:space="preserve">Linha de produção seleciona componentes a serem fixados</t>
+    <t xml:space="preserve">Linha de produção seleciona componentes</t>
   </si>
   <si>
     <t xml:space="preserve">(x)5</t>
@@ -139,73 +139,19 @@
     <t xml:space="preserve">(x)10</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Controle de qualidade</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> coloca subcomponentes testados</t>
-    </r>
+    <t xml:space="preserve">Controle de qualidade coloca subcomponentes testados</t>
   </si>
   <si>
     <t xml:space="preserve">(x)11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Controle de qualidade</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> termina montagem da maquina</t>
-    </r>
+    <t xml:space="preserve">Controle de qualidade termina montagem da maquina</t>
   </si>
   <si>
     <t xml:space="preserve">(x)12</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Controle de qualidade</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> seleciona maquina montada</t>
-    </r>
+    <t xml:space="preserve">Controle de qualidade seleciona maquina montada</t>
   </si>
   <si>
     <t xml:space="preserve">(x)13</t>
@@ -249,7 +195,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,12 +283,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -448,7 +388,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,10 +413,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,10 +515,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -676,11 +608,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.43"/>
@@ -726,7 +658,7 @@
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -740,460 +672,460 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="n">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="15" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="n">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="15" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="20" t="n">
+      <c r="A8" s="18"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="25" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="20" t="n">
+      <c r="A9" s="18"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="26" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="20" t="n">
+      <c r="A10" s="18"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="26" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="20" t="n">
+      <c r="A11" s="18"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="26" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="20" t="n">
+      <c r="C13" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20" t="n">
+      <c r="C14" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="25" t="s">
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="20" t="n">
+      <c r="C16" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="25" t="s">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="20" t="n">
+      <c r="C17" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="25" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="14"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="20" t="n">
+      <c r="C18" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="25" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="20" t="n">
+      <c r="C19" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="25" t="s">
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="20" t="n">
+      <c r="C21" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="20" t="n">
+      <c r="C22" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="25" t="s">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="32"/>
+      <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="20" t="n">
+      <c r="C24" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="10"/>
+      <c r="F24" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="20" t="n">
+      <c r="A25" s="33"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="25" t="s">
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35"/>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="20"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="36"/>
+      <c r="D28" s="34"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>